<commit_message>
working ice bath code
</commit_message>
<xml_diff>
--- a/OutputFiles/hobo_icebathcalib_022123.xlsx
+++ b/OutputFiles/hobo_icebathcalib_022123.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,109 +360,149 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Logger_Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Serial_Number</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>avg_temp</t>
-        </is>
-      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>sd_temp</t>
+          <t>avg_ice_bath_temp</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>sd_ice_bath_temp</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>M-10</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>10009526</t>
         </is>
       </c>
-      <c r="B2">
-        <v>6.679806451612904</v>
-      </c>
       <c r="C2">
-        <v>10.07836919486268</v>
+        <v>0.3253076923076923</v>
+      </c>
+      <c r="D2">
+        <v>1.10393307350094</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>M-07</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>10081490</t>
         </is>
       </c>
-      <c r="B3">
-        <v>8.515033333333333</v>
-      </c>
       <c r="C3">
-        <v>8.587777932995053</v>
+        <v>3.505615384615385</v>
+      </c>
+      <c r="D3">
+        <v>1.0772885359752</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>M-08</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>10081491</t>
         </is>
       </c>
-      <c r="B4">
-        <v>7.013709677419355</v>
-      </c>
       <c r="C4">
-        <v>9.97686353918755</v>
+        <v>0.5703076923076923</v>
+      </c>
+      <c r="D4">
+        <v>1.620001923075782</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>M-09</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>10081493</t>
         </is>
       </c>
-      <c r="B5">
-        <v>7.029892857142857</v>
-      </c>
       <c r="C5">
-        <v>9.373224570015758</v>
+        <v>1.280538461538462</v>
+      </c>
+      <c r="D5">
+        <v>1.048488325748441</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>M-11</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>20679351</t>
         </is>
       </c>
-      <c r="B6">
-        <v>6.270965517241379</v>
-      </c>
       <c r="C6">
-        <v>9.656961853956371</v>
+        <v>0.7213076923076923</v>
+      </c>
+      <c r="D6">
+        <v>1.273060903532335</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>M-06</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>20679352</t>
         </is>
       </c>
-      <c r="B7">
-        <v>7.599</v>
-      </c>
       <c r="C7">
-        <v>10.20649389738804</v>
+        <v>0.5387692307692308</v>
+      </c>
+      <c r="D7">
+        <v>1.042164666599138</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>9995411,</t>
-        </is>
-      </c>
-      <c r="B8">
-        <v>7.769121212121212</v>
+          <t>M-12</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>9995411</t>
+        </is>
       </c>
       <c r="C8">
-        <v>10.37303600313565</v>
+        <v>0.4598461538461538</v>
+      </c>
+      <c r="D8">
+        <v>1.188771764340114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
temps still look high
</commit_message>
<xml_diff>
--- a/OutputFiles/hobo_icebathcalib_022123.xlsx
+++ b/OutputFiles/hobo_icebathcalib_022123.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -391,10 +391,10 @@
         </is>
       </c>
       <c r="C2">
-        <v>0.3253076923076923</v>
+        <v>0.5757868852459016</v>
       </c>
       <c r="D2">
-        <v>1.10393307350094</v>
+        <v>0.2305781946003061</v>
       </c>
     </row>
     <row r="3">
@@ -409,10 +409,10 @@
         </is>
       </c>
       <c r="C3">
-        <v>3.505615384615385</v>
+        <v>0.5560491803278689</v>
       </c>
       <c r="D3">
-        <v>1.0772885359752</v>
+        <v>0.08526320547369935</v>
       </c>
     </row>
     <row r="4">
@@ -427,10 +427,10 @@
         </is>
       </c>
       <c r="C4">
-        <v>0.5703076923076923</v>
+        <v>0.3573934426229509</v>
       </c>
       <c r="D4">
-        <v>1.620001923075782</v>
+        <v>0.05498553709492602</v>
       </c>
     </row>
     <row r="5">
@@ -445,64 +445,622 @@
         </is>
       </c>
       <c r="C5">
-        <v>1.280538461538462</v>
+        <v>0.5017049180327869</v>
       </c>
       <c r="D5">
-        <v>1.048488325748441</v>
+        <v>0.1972142104635038</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>M-11</t>
+          <t>M-13</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>20679351</t>
+          <t>20334331</t>
         </is>
       </c>
       <c r="C6">
-        <v>0.7213076923076923</v>
+        <v>0.449344262295082</v>
       </c>
       <c r="D6">
-        <v>1.273060903532335</v>
+        <v>0.1025174595285931</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>M-06</t>
+          <t>M-14</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>20679352</t>
+          <t>20334332</t>
         </is>
       </c>
       <c r="C7">
-        <v>0.5387692307692308</v>
+        <v>0.350016393442623</v>
       </c>
       <c r="D7">
-        <v>1.042164666599138</v>
+        <v>0.1025193464349174</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>M-15</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>20334333</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>0.5847213114754098</v>
+      </c>
+      <c r="D8">
+        <v>0.1446090282045052</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>M-16</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>20334334</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>0.6171803278688525</v>
+      </c>
+      <c r="D9">
+        <v>0.1941114377702253</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>M-20</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>20334335</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>0.1498524590163934</v>
+      </c>
+      <c r="D10">
+        <v>0.2157571038664833</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>M-17</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>20334339</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>0.2730491803278688</v>
+      </c>
+      <c r="D11">
+        <v>0.2801661070525548</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>M-18</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>20590215</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>0.5594098360655737</v>
+      </c>
+      <c r="D12">
+        <v>0.1772193910617741</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>M-19</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>20590219</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>0.2338196721311475</v>
+      </c>
+      <c r="D13">
+        <v>0.01421209367255146</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>M-11</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>20679351</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>0.3138852459016394</v>
+      </c>
+      <c r="D14">
+        <v>0.04923213664557456</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>M-06</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>20679352</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>0.2447377049180328</v>
+      </c>
+      <c r="D15">
+        <v>0.0410267805379788</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>M-21</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>21098309</t>
+        </is>
+      </c>
+      <c r="C16">
+        <v>0.2338196721311475</v>
+      </c>
+      <c r="D16">
+        <v>0.02475244647620467</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>M-23</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>21098311</t>
+        </is>
+      </c>
+      <c r="C17">
+        <v>0.5630655737704918</v>
+      </c>
+      <c r="D17">
+        <v>0.1785346715955997</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>M-24</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>21098312</t>
+        </is>
+      </c>
+      <c r="C18">
+        <v>0.2731803278688524</v>
+      </c>
+      <c r="D18">
+        <v>0.2495352018050574</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>M-39</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>21098313</t>
+        </is>
+      </c>
+      <c r="C19">
+        <v>0.5378196721311476</v>
+      </c>
+      <c r="D19">
+        <v>0.1195858838097431</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>M-25</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>21098314</t>
+        </is>
+      </c>
+      <c r="C20">
+        <v>0.6773114754098361</v>
+      </c>
+      <c r="D20">
+        <v>0.08779228154828622</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>M-26</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>21098315</t>
+        </is>
+      </c>
+      <c r="C21">
+        <v>0.6317213114754099</v>
+      </c>
+      <c r="D21">
+        <v>0.1914634108776871</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>M-27</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>21098316</t>
+        </is>
+      </c>
+      <c r="C22">
+        <v>0.4711147540983607</v>
+      </c>
+      <c r="D22">
+        <v>0.09264881693086277</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>M-28</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>21098317</t>
+        </is>
+      </c>
+      <c r="C23">
+        <v>0.2882295081967213</v>
+      </c>
+      <c r="D23">
+        <v>0.1100253597195699</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>M-30</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>21098319</t>
+        </is>
+      </c>
+      <c r="C24">
+        <v>0.4891147540983606</v>
+      </c>
+      <c r="D24">
+        <v>0.08467410040082222</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>M-31</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>21098320</t>
+        </is>
+      </c>
+      <c r="C25">
+        <v>0.6627377049180327</v>
+      </c>
+      <c r="D25">
+        <v>0.1095317155955821</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>M-32</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>21098321</t>
+        </is>
+      </c>
+      <c r="C26">
+        <v>0.5486393442622951</v>
+      </c>
+      <c r="D26">
+        <v>0.1355202362240765</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>M-33</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>21098322</t>
+        </is>
+      </c>
+      <c r="C27">
+        <v>0.4294918032786885</v>
+      </c>
+      <c r="D27">
+        <v>0.1479999575395006</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>M-34</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>21098323</t>
+        </is>
+      </c>
+      <c r="C28">
+        <v>0.6499180327868852</v>
+      </c>
+      <c r="D28">
+        <v>0.1680432776679832</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>M-35</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>21098324</t>
+        </is>
+      </c>
+      <c r="C29">
+        <v>0.6392950819672131</v>
+      </c>
+      <c r="D29">
+        <v>0.07695633919357461</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>M-36</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>21098325</t>
+        </is>
+      </c>
+      <c r="C30">
+        <v>0.4168688524590164</v>
+      </c>
+      <c r="D30">
+        <v>0.1592794687972303</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>M-37</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>21098326</t>
+        </is>
+      </c>
+      <c r="C31">
+        <v>0.3627704918032787</v>
+      </c>
+      <c r="D31">
+        <v>0.06825696385537594</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>M-38</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>21098327</t>
+        </is>
+      </c>
+      <c r="C32">
+        <v>0.5341311475409836</v>
+      </c>
+      <c r="D32">
+        <v>0.2103376234699692</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>M-40</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>21398136</t>
+        </is>
+      </c>
+      <c r="C33">
+        <v>0.5829508196721311</v>
+      </c>
+      <c r="D33">
+        <v>0.1214637704872675</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>M-41</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>21398137</t>
+        </is>
+      </c>
+      <c r="C34">
+        <v>0.5035737704918033</v>
+      </c>
+      <c r="D34">
+        <v>0.1093956822756111</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>M-42</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>21398138</t>
+        </is>
+      </c>
+      <c r="C35">
+        <v>0.367672131147541</v>
+      </c>
+      <c r="D35">
+        <v>0.2181878182752553</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>M-43</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>21398139</t>
+        </is>
+      </c>
+      <c r="C36">
+        <v>0.5594426229508197</v>
+      </c>
+      <c r="D36">
+        <v>0.1502582803697425</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>M-44</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>21398140</t>
+        </is>
+      </c>
+      <c r="C37">
+        <v>0.416983606557377</v>
+      </c>
+      <c r="D37">
+        <v>0.09375633166232537</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>M-45</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>21398141</t>
+        </is>
+      </c>
+      <c r="C38">
+        <v>0.3735409836065574</v>
+      </c>
+      <c r="D38">
+        <v>0.1159622889521261</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
           <t>M-12</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B39" t="inlineStr">
         <is>
           <t>9995411</t>
         </is>
       </c>
-      <c r="C8">
-        <v>0.4598461538461538</v>
-      </c>
-      <c r="D8">
-        <v>1.188771764340114</v>
+      <c r="C39">
+        <v>0.59</v>
+      </c>
+      <c r="D39">
+        <v>0.2011504412125412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>